<commit_message>
Recalced the Batch NN tests to get std deviation. Fixed the LOO tests to use the batch method. Other small things.
</commit_message>
<xml_diff>
--- a/ClassifierTesterResults/Batch/hfimaginary-Parsed_Results_nn.xlsx
+++ b/ClassifierTesterResults/Batch/hfimaginary-Parsed_Results_nn.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="759">
   <si>
     <t>layout</t>
   </si>
@@ -133,34 +133,34 @@
     <t xml:space="preserve">100 </t>
   </si>
   <si>
-    <t>0.5740740740740741</t>
-  </si>
-  <si>
-    <t>0.6552730696798493</t>
-  </si>
-  <si>
-    <t>0.6595572584078332</t>
-  </si>
-  <si>
-    <t>0.7002489884842826</t>
-  </si>
-  <si>
-    <t>0.6936789797947517</t>
-  </si>
-  <si>
-    <t>0.6808980085222367</t>
-  </si>
-  <si>
-    <t>0.69585326953748</t>
-  </si>
-  <si>
-    <t>0.7225853990621318</t>
-  </si>
-  <si>
-    <t>0.7258460630474324</t>
-  </si>
-  <si>
-    <t>0.7334166733260802</t>
+    <t>0.5593103448275862</t>
+  </si>
+  <si>
+    <t>0.6710734463276836</t>
+  </si>
+  <si>
+    <t>0.7074573449854349</t>
+  </si>
+  <si>
+    <t>0.719313372487591</t>
+  </si>
+  <si>
+    <t>0.6865459044790894</t>
+  </si>
+  <si>
+    <t>0.6772173168308976</t>
+  </si>
+  <si>
+    <t>0.706072175381515</t>
+  </si>
+  <si>
+    <t>0.705208099911451</t>
+  </si>
+  <si>
+    <t>0.714135813826603</t>
+  </si>
+  <si>
+    <t>0.7250550118939005</t>
   </si>
   <si>
     <t>0.5504980842911877</t>
@@ -223,7 +223,34 @@
     <t>0.6444365500360804</t>
   </si>
   <si>
-    <t>0.0</t>
+    <t>0.02850368715005569</t>
+  </si>
+  <si>
+    <t>0.02471950669037932</t>
+  </si>
+  <si>
+    <t>0.03051139248884247</t>
+  </si>
+  <si>
+    <t>0.020303463488732437</t>
+  </si>
+  <si>
+    <t>0.03310639632593836</t>
+  </si>
+  <si>
+    <t>0.03348587238826618</t>
+  </si>
+  <si>
+    <t>0.024675180942976525</t>
+  </si>
+  <si>
+    <t>0.017892601798075735</t>
+  </si>
+  <si>
+    <t>0.01624544803352867</t>
+  </si>
+  <si>
+    <t>0.008357407469267055</t>
   </si>
   <si>
     <t>0.06812057972500041</t>
@@ -286,34 +313,34 @@
     <t>0.01602893242813989</t>
   </si>
   <si>
-    <t>0.5568128089404686</t>
-  </si>
-  <si>
-    <t>0.6055899328737628</t>
-  </si>
-  <si>
-    <t>0.6532749358620006</t>
-  </si>
-  <si>
-    <t>0.7356751213795413</t>
-  </si>
-  <si>
-    <t>0.6790585628870383</t>
-  </si>
-  <si>
-    <t>0.6877706892091493</t>
-  </si>
-  <si>
-    <t>0.6878541040158184</t>
-  </si>
-  <si>
-    <t>0.7112248030919567</t>
-  </si>
-  <si>
-    <t>0.7127067349087918</t>
-  </si>
-  <si>
-    <t>0.719428869127578</t>
+    <t>0.7363602805463271</t>
+  </si>
+  <si>
+    <t>0.6212249783561854</t>
+  </si>
+  <si>
+    <t>0.6716979014700931</t>
+  </si>
+  <si>
+    <t>0.7101068780623601</t>
+  </si>
+  <si>
+    <t>0.657454417841586</t>
+  </si>
+  <si>
+    <t>0.7070171312933047</t>
+  </si>
+  <si>
+    <t>0.7019822884534853</t>
+  </si>
+  <si>
+    <t>0.6972849620092931</t>
+  </si>
+  <si>
+    <t>0.6945357813575596</t>
+  </si>
+  <si>
+    <t>0.7018490754950536</t>
   </si>
   <si>
     <t>0.6036832718157072</t>
@@ -376,34 +403,34 @@
     <t>0.6229757318565782</t>
   </si>
   <si>
-    <t>0.5683958020989506</t>
-  </si>
-  <si>
-    <t>0.6848404255319149</t>
-  </si>
-  <si>
-    <t>0.6583075206263834</t>
-  </si>
-  <si>
-    <t>0.6845104504354733</t>
-  </si>
-  <si>
-    <t>0.699080182102327</t>
-  </si>
-  <si>
-    <t>0.6793518862890315</t>
-  </si>
-  <si>
-    <t>0.7028361166908063</t>
-  </si>
-  <si>
-    <t>0.7270445325178704</t>
-  </si>
-  <si>
-    <t>0.7319751946829411</t>
-  </si>
-  <si>
-    <t>0.7418550926077931</t>
+    <t>0.5412121212121213</t>
+  </si>
+  <si>
+    <t>0.6970945347186674</t>
+  </si>
+  <si>
+    <t>0.7232685617787785</t>
+  </si>
+  <si>
+    <t>0.7257140983441207</t>
+  </si>
+  <si>
+    <t>0.6970758370836314</t>
+  </si>
+  <si>
+    <t>0.6687264927361136</t>
+  </si>
+  <si>
+    <t>0.7110904585670724</t>
+  </si>
+  <si>
+    <t>0.7111024459501413</t>
+  </si>
+  <si>
+    <t>0.7236446091122916</t>
+  </si>
+  <si>
+    <t>0.7364939947836892</t>
   </si>
   <si>
     <t>0.5573276905146685</t>
@@ -466,34 +493,34 @@
     <t>0.6544091414743075</t>
   </si>
   <si>
-    <t>0.5455430399109998</t>
-  </si>
-  <si>
-    <t>0.6396074521910643</t>
-  </si>
-  <si>
-    <t>0.6556749930976044</t>
-  </si>
-  <si>
-    <t>0.7091360542514841</t>
-  </si>
-  <si>
-    <t>0.6883284616359292</t>
-  </si>
-  <si>
-    <t>0.6831858257275458</t>
-  </si>
-  <si>
-    <t>0.6947418437397843</t>
-  </si>
-  <si>
-    <t>0.7189230129694035</t>
-  </si>
-  <si>
-    <t>0.7213298503647497</t>
-  </si>
-  <si>
-    <t>0.729647873997409</t>
+    <t>0.6166233950229429</t>
+  </si>
+  <si>
+    <t>0.6549510867931334</t>
+  </si>
+  <si>
+    <t>0.6927514629873976</t>
+  </si>
+  <si>
+    <t>0.7153641066689314</t>
+  </si>
+  <si>
+    <t>0.6760675037495496</t>
+  </si>
+  <si>
+    <t>0.6860338014041466</t>
+  </si>
+  <si>
+    <t>0.7056056874696713</t>
+  </si>
+  <si>
+    <t>0.7027818038084341</t>
+  </si>
+  <si>
+    <t>0.7086358563429864</t>
+  </si>
+  <si>
+    <t>0.7182272306436291</t>
   </si>
   <si>
     <t>0.5580621325730275</t>
@@ -556,34 +583,34 @@
     <t>0.6364964332961917</t>
   </si>
   <si>
-    <t>0.5724314203860489</t>
-  </si>
-  <si>
-    <t>0.6558449337109867</t>
-  </si>
-  <si>
-    <t>0.659553781190825</t>
-  </si>
-  <si>
-    <t>0.7005124374863795</t>
-  </si>
-  <si>
-    <t>0.6935094989934014</t>
-  </si>
-  <si>
-    <t>0.6809812466804485</t>
-  </si>
-  <si>
-    <t>0.696020066084678</t>
-  </si>
-  <si>
-    <t>0.7226108112623283</t>
-  </si>
-  <si>
-    <t>0.7259150230519097</t>
-  </si>
-  <si>
-    <t>0.7335662778307809</t>
+    <t>0.5597963018893252</t>
+  </si>
+  <si>
+    <t>0.6715378482049628</t>
+  </si>
+  <si>
+    <t>0.7071594228485024</t>
+  </si>
+  <si>
+    <t>0.7199910403824115</t>
+  </si>
+  <si>
+    <t>0.6865636206021704</t>
+  </si>
+  <si>
+    <t>0.6773141676382389</t>
+  </si>
+  <si>
+    <t>0.7061389746764182</t>
+  </si>
+  <si>
+    <t>0.7053660393798005</t>
+  </si>
+  <si>
+    <t>0.7141392747067533</t>
+  </si>
+  <si>
+    <t>0.7249480459441296</t>
   </si>
   <si>
     <t>0.5538285043556864</t>
@@ -646,31 +673,34 @@
     <t>0.6444739803918156</t>
   </si>
   <si>
-    <t>0.6533584431889518</t>
-  </si>
-  <si>
-    <t>0.659855257556407</t>
-  </si>
-  <si>
-    <t>0.7039293495175848</t>
-  </si>
-  <si>
-    <t>0.7018735130144527</t>
-  </si>
-  <si>
-    <t>0.6765003757064916</t>
-  </si>
-  <si>
-    <t>0.705404926457558</t>
-  </si>
-  <si>
-    <t>0.7258560171205591</t>
-  </si>
-  <si>
-    <t>0.7324519530449453</t>
-  </si>
-  <si>
-    <t>0.7497971460023471</t>
+    <t>0.5655172413793104</t>
+  </si>
+  <si>
+    <t>0.6522598870056496</t>
+  </si>
+  <si>
+    <t>0.6881148564294632</t>
+  </si>
+  <si>
+    <t>0.7316647740887284</t>
+  </si>
+  <si>
+    <t>0.7012274189557041</t>
+  </si>
+  <si>
+    <t>0.7037141330521505</t>
+  </si>
+  <si>
+    <t>0.7191345404623313</t>
+  </si>
+  <si>
+    <t>0.7151370605848935</t>
+  </si>
+  <si>
+    <t>0.7188404806341671</t>
+  </si>
+  <si>
+    <t>0.7321927353471728</t>
   </si>
   <si>
     <t>0.5075095785440613</t>
@@ -733,6 +763,36 @@
     <t>0.6609042487565195</t>
   </si>
   <si>
+    <t>0.058882793702866566</t>
+  </si>
+  <si>
+    <t>0.03383992671412854</t>
+  </si>
+  <si>
+    <t>0.02760104344034561</t>
+  </si>
+  <si>
+    <t>0.03833835533969087</t>
+  </si>
+  <si>
+    <t>0.03396710375981088</t>
+  </si>
+  <si>
+    <t>0.025306839369230984</t>
+  </si>
+  <si>
+    <t>0.011610477394811535</t>
+  </si>
+  <si>
+    <t>0.021016663185234142</t>
+  </si>
+  <si>
+    <t>0.007468974882147412</t>
+  </si>
+  <si>
+    <t>0.018500226962007295</t>
+  </si>
+  <si>
     <t>0.05439350131338672</t>
   </si>
   <si>
@@ -793,34 +853,34 @@
     <t>0.01969015209819078</t>
   </si>
   <si>
-    <t>0.46369009241349674</t>
-  </si>
-  <si>
-    <t>0.6830176048055873</t>
-  </si>
-  <si>
-    <t>0.630633158991368</t>
-  </si>
-  <si>
-    <t>0.714841788046208</t>
-  </si>
-  <si>
-    <t>0.7119634849455476</t>
-  </si>
-  <si>
-    <t>0.6826050281085623</t>
-  </si>
-  <si>
-    <t>0.7056653346021514</t>
-  </si>
-  <si>
-    <t>0.7424464959143192</t>
-  </si>
-  <si>
-    <t>0.7028160012632688</t>
-  </si>
-  <si>
-    <t>0.7432737484100468</t>
+    <t>0.8432436162870947</t>
+  </si>
+  <si>
+    <t>0.6416050392762971</t>
+  </si>
+  <si>
+    <t>0.6325328245988104</t>
+  </si>
+  <si>
+    <t>0.7250790317974891</t>
+  </si>
+  <si>
+    <t>0.6522762437474826</t>
+  </si>
+  <si>
+    <t>0.6859912751060904</t>
+  </si>
+  <si>
+    <t>0.7203140985099634</t>
+  </si>
+  <si>
+    <t>0.7289084945575957</t>
+  </si>
+  <si>
+    <t>0.7203753248946637</t>
+  </si>
+  <si>
+    <t>0.7193688028160656</t>
   </si>
   <si>
     <t>0.7173264293523314</t>
@@ -883,34 +943,34 @@
     <t>0.6359405499995701</t>
   </si>
   <si>
-    <t>0.5919191919191918</t>
-  </si>
-  <si>
-    <t>0.651835816241305</t>
-  </si>
-  <si>
-    <t>0.6639194937234153</t>
-  </si>
-  <si>
-    <t>0.6964887093473798</t>
-  </si>
-  <si>
-    <t>0.6963913530996941</t>
-  </si>
-  <si>
-    <t>0.6750567456376791</t>
-  </si>
-  <si>
-    <t>0.7079555278901685</t>
-  </si>
-  <si>
-    <t>0.7192452961364076</t>
-  </si>
-  <si>
-    <t>0.7476191755172202</t>
-  </si>
-  <si>
-    <t>0.7553516369529824</t>
+    <t>0.5468371006502138</t>
+  </si>
+  <si>
+    <t>0.6625460340797037</t>
+  </si>
+  <si>
+    <t>0.7183889545193229</t>
+  </si>
+  <si>
+    <t>0.7335070717735525</t>
+  </si>
+  <si>
+    <t>0.7218724501149766</t>
+  </si>
+  <si>
+    <t>0.714395615696616</t>
+  </si>
+  <si>
+    <t>0.721330308964345</t>
+  </si>
+  <si>
+    <t>0.7107651774624497</t>
+  </si>
+  <si>
+    <t>0.7190441642433634</t>
+  </si>
+  <si>
+    <t>0.7387616571264385</t>
   </si>
   <si>
     <t>0.5115547149839669</t>
@@ -973,34 +1033,34 @@
     <t>0.670672007085962</t>
   </si>
   <si>
-    <t>0.4817331677796794</t>
-  </si>
-  <si>
-    <t>0.6659153376827353</t>
-  </si>
-  <si>
-    <t>0.6440268910048216</t>
-  </si>
-  <si>
-    <t>0.7055448800875809</t>
-  </si>
-  <si>
-    <t>0.7040021826708646</t>
-  </si>
-  <si>
-    <t>0.6786435949934582</t>
-  </si>
-  <si>
-    <t>0.7067013482491467</t>
-  </si>
-  <si>
-    <t>0.7298343317890797</t>
-  </si>
-  <si>
-    <t>0.7234957015868452</t>
-  </si>
-  <si>
-    <t>0.748282361803342</t>
+    <t>0.6565619288788745</t>
+  </si>
+  <si>
+    <t>0.6494504459464976</t>
+  </si>
+  <si>
+    <t>0.6637263917771673</t>
+  </si>
+  <si>
+    <t>0.7272856588074703</t>
+  </si>
+  <si>
+    <t>0.681167834275832</t>
+  </si>
+  <si>
+    <t>0.6986241960731304</t>
+  </si>
+  <si>
+    <t>0.7198916763340433</t>
+  </si>
+  <si>
+    <t>0.7188854690202421</t>
+  </si>
+  <si>
+    <t>0.7194312775091343</t>
+  </si>
+  <si>
+    <t>0.7284235723351331</t>
   </si>
   <si>
     <t>0.5807264540662</t>
@@ -1063,34 +1123,34 @@
     <t>0.6511435803786563</t>
   </si>
   <si>
-    <t>0.5759824090498745</t>
-  </si>
-  <si>
-    <t>0.6532827564181269</t>
-  </si>
-  <si>
-    <t>0.6598871416758855</t>
-  </si>
-  <si>
-    <t>0.7039799441995497</t>
-  </si>
-  <si>
-    <t>0.7019456265876229</t>
-  </si>
-  <si>
-    <t>0.6765280682230753</t>
-  </si>
-  <si>
-    <t>0.7054155482069041</t>
-  </si>
-  <si>
-    <t>0.7263020367877258</t>
-  </si>
-  <si>
-    <t>0.7326958224115879</t>
-  </si>
-  <si>
-    <t>0.7500116119277958</t>
+    <t>0.569639484911224</t>
+  </si>
+  <si>
+    <t>0.6520707477293135</t>
+  </si>
+  <si>
+    <t>0.6877834781081887</t>
+  </si>
+  <si>
+    <t>0.7316681525672208</t>
+  </si>
+  <si>
+    <t>0.7011182987652456</t>
+  </si>
+  <si>
+    <t>0.7038600055152843</t>
+  </si>
+  <si>
+    <t>0.7191499834581518</t>
+  </si>
+  <si>
+    <t>0.715259936975691</t>
+  </si>
+  <si>
+    <t>0.7188472222168374</t>
+  </si>
+  <si>
+    <t>0.7321491030750172</t>
   </si>
   <si>
     <t>0.5144795172366543</t>
@@ -1153,34 +1213,34 @@
     <t>0.6608967474811489</t>
   </si>
   <si>
-    <t>0.5222222222222221</t>
-  </si>
-  <si>
-    <t>0.5842749529190208</t>
-  </si>
-  <si>
-    <t>0.6533844189016603</t>
-  </si>
-  <si>
-    <t>0.6600918145035791</t>
-  </si>
-  <si>
-    <t>0.6431230469443557</t>
-  </si>
-  <si>
-    <t>0.6597931047357686</t>
-  </si>
-  <si>
-    <t>0.6756588440798966</t>
-  </si>
-  <si>
-    <t>0.7026690512168966</t>
-  </si>
-  <si>
-    <t>0.6953843117866235</t>
-  </si>
-  <si>
-    <t>0.7188955264549984</t>
+    <t>0.5436781609195401</t>
+  </si>
+  <si>
+    <t>0.612015065913371</t>
+  </si>
+  <si>
+    <t>0.6465251768622555</t>
+  </si>
+  <si>
+    <t>0.6254264530145953</t>
+  </si>
+  <si>
+    <t>0.67278000494927</t>
+  </si>
+  <si>
+    <t>0.6631334469675394</t>
+  </si>
+  <si>
+    <t>0.6697291552370601</t>
+  </si>
+  <si>
+    <t>0.6674815073488508</t>
+  </si>
+  <si>
+    <t>0.6894025798731607</t>
+  </si>
+  <si>
+    <t>0.7002335120542911</t>
   </si>
   <si>
     <t>0.5120306513409961</t>
@@ -1243,6 +1303,36 @@
     <t>0.5972189580935275</t>
   </si>
   <si>
+    <t>0.011552851904818015</t>
+  </si>
+  <si>
+    <t>0.036790637708713644</t>
+  </si>
+  <si>
+    <t>0.037246100647784976</t>
+  </si>
+  <si>
+    <t>0.028200880193587925</t>
+  </si>
+  <si>
+    <t>0.05333908158043765</t>
+  </si>
+  <si>
+    <t>0.05187377832867913</t>
+  </si>
+  <si>
+    <t>0.02855917780779681</t>
+  </si>
+  <si>
+    <t>0.023261915289272274</t>
+  </si>
+  <si>
+    <t>0.03609927338570964</t>
+  </si>
+  <si>
+    <t>0.03986626181618877</t>
+  </si>
+  <si>
     <t>0.022676814154704027</t>
   </si>
   <si>
@@ -1303,34 +1393,34 @@
     <t>0.02056608089053618</t>
   </si>
   <si>
-    <t>0.4971953578336558</t>
-  </si>
-  <si>
-    <t>0.7688604823680544</t>
-  </si>
-  <si>
-    <t>0.6600019843800938</t>
-  </si>
-  <si>
-    <t>0.7539866901054747</t>
-  </si>
-  <si>
-    <t>0.6716848174247277</t>
-  </si>
-  <si>
-    <t>0.7279906202798895</t>
-  </si>
-  <si>
-    <t>0.7288386864314383</t>
-  </si>
-  <si>
-    <t>0.7606643913736527</t>
-  </si>
-  <si>
-    <t>0.6746628171108914</t>
-  </si>
-  <si>
-    <t>0.765017336667265</t>
+    <t>0.5287001460510055</t>
+  </si>
+  <si>
+    <t>0.7265686349412338</t>
+  </si>
+  <si>
+    <t>0.665480866344967</t>
+  </si>
+  <si>
+    <t>0.7046251267726775</t>
+  </si>
+  <si>
+    <t>0.7172119299221069</t>
+  </si>
+  <si>
+    <t>0.6951257253800788</t>
+  </si>
+  <si>
+    <t>0.7436397251762237</t>
+  </si>
+  <si>
+    <t>0.6468974443496329</t>
+  </si>
+  <si>
+    <t>0.7479973406702664</t>
+  </si>
+  <si>
+    <t>0.7193832612473585</t>
   </si>
   <si>
     <t>0.6746453272075543</t>
@@ -1393,34 +1483,34 @@
     <t>0.516562250088141</t>
   </si>
   <si>
-    <t>0.5444270015698587</t>
-  </si>
-  <si>
-    <t>0.5743061194360375</t>
-  </si>
-  <si>
-    <t>0.6464574226937579</t>
-  </si>
-  <si>
-    <t>0.6357752407859687</t>
-  </si>
-  <si>
-    <t>0.632909090909091</t>
-  </si>
-  <si>
-    <t>0.642631968932022</t>
-  </si>
-  <si>
-    <t>0.6616043260240166</t>
-  </si>
-  <si>
-    <t>0.6814972025163811</t>
-  </si>
-  <si>
-    <t>0.704973181729604</t>
-  </si>
-  <si>
-    <t>0.7024654918853628</t>
+    <t>0.5520985719261582</t>
+  </si>
+  <si>
+    <t>0.598441364525702</t>
+  </si>
+  <si>
+    <t>0.6443690318144747</t>
+  </si>
+  <si>
+    <t>0.6081742316003926</t>
+  </si>
+  <si>
+    <t>0.656529173441981</t>
+  </si>
+  <si>
+    <t>0.6550847194783557</t>
+  </si>
+  <si>
+    <t>0.6596364139203478</t>
+  </si>
+  <si>
+    <t>0.6807356279034196</t>
+  </si>
+  <si>
+    <t>0.6706737179464435</t>
+  </si>
+  <si>
+    <t>0.6940116206618696</t>
   </si>
   <si>
     <t>0.5111447542038874</t>
@@ -1483,34 +1573,34 @@
     <t>0.6250041657478829</t>
   </si>
   <si>
-    <t>0.4815924219150027</t>
-  </si>
-  <si>
-    <t>0.6502548448353714</t>
-  </si>
-  <si>
-    <t>0.6513046569142811</t>
-  </si>
-  <si>
-    <t>0.6891149822299455</t>
-  </si>
-  <si>
-    <t>0.6512625170098364</t>
-  </si>
-  <si>
-    <t>0.6814587573907144</t>
-  </si>
-  <si>
-    <t>0.6934118124773075</t>
-  </si>
-  <si>
-    <t>0.7187380177437078</t>
-  </si>
-  <si>
-    <t>0.6889111821437957</t>
-  </si>
-  <si>
-    <t>0.7310484039660293</t>
+    <t>0.5133556560453416</t>
+  </si>
+  <si>
+    <t>0.6490758954868697</t>
+  </si>
+  <si>
+    <t>0.6493182111814986</t>
+  </si>
+  <si>
+    <t>0.6500183859514931</t>
+  </si>
+  <si>
+    <t>0.6848729159293359</t>
+  </si>
+  <si>
+    <t>0.6735241857960061</t>
+  </si>
+  <si>
+    <t>0.6920107735410514</t>
+  </si>
+  <si>
+    <t>0.6541988449919257</t>
+  </si>
+  <si>
+    <t>0.7066362986317744</t>
+  </si>
+  <si>
+    <t>0.697870997490169</t>
   </si>
   <si>
     <t>0.5722706342399739</t>
@@ -1573,34 +1663,34 @@
     <t>0.5506059482115397</t>
   </si>
   <si>
-    <t>0.5192638961957853</t>
-  </si>
-  <si>
-    <t>0.5828891099015165</t>
-  </si>
-  <si>
-    <t>0.6533486419652524</t>
-  </si>
-  <si>
-    <t>0.6607521030390949</t>
-  </si>
-  <si>
-    <t>0.6431537353686264</t>
-  </si>
-  <si>
-    <t>0.6597231110215568</t>
-  </si>
-  <si>
-    <t>0.6753818023192121</t>
-  </si>
-  <si>
-    <t>0.7028660030307917</t>
-  </si>
-  <si>
-    <t>0.6955473062523536</t>
-  </si>
-  <si>
-    <t>0.7193621064334752</t>
+    <t>0.5459409821164118</t>
+  </si>
+  <si>
+    <t>0.61156032146146</t>
+  </si>
+  <si>
+    <t>0.646726321677575</t>
+  </si>
+  <si>
+    <t>0.6257536439457088</t>
+  </si>
+  <si>
+    <t>0.6729719342320569</t>
+  </si>
+  <si>
+    <t>0.6631795836719288</t>
+  </si>
+  <si>
+    <t>0.6693617391369022</t>
+  </si>
+  <si>
+    <t>0.6672569684477915</t>
+  </si>
+  <si>
+    <t>0.6893323363595311</t>
+  </si>
+  <si>
+    <t>0.7002859598958813</t>
   </si>
   <si>
     <t>0.5148262181779811</t>
@@ -1663,34 +1753,34 @@
     <t>0.59804342790529</t>
   </si>
   <si>
-    <t>0.5333333333333333</t>
-  </si>
-  <si>
-    <t>0.6201192718141871</t>
-  </si>
-  <si>
-    <t>0.6173690932311622</t>
-  </si>
-  <si>
-    <t>0.6369125427948957</t>
-  </si>
-  <si>
-    <t>0.6208894171016653</t>
-  </si>
-  <si>
-    <t>0.667804287254449</t>
-  </si>
-  <si>
-    <t>0.6640414166729957</t>
-  </si>
-  <si>
-    <t>0.6803549863151699</t>
-  </si>
-  <si>
-    <t>0.6978352036419784</t>
-  </si>
-  <si>
-    <t>0.703287059473109</t>
+    <t>0.5168582375478927</t>
+  </si>
+  <si>
+    <t>0.5964218455743879</t>
+  </si>
+  <si>
+    <t>0.6533666250520184</t>
+  </si>
+  <si>
+    <t>0.6571616461337919</t>
+  </si>
+  <si>
+    <t>0.6572096015837664</t>
+  </si>
+  <si>
+    <t>0.6623093226757831</t>
+  </si>
+  <si>
+    <t>0.6987839788624235</t>
+  </si>
+  <si>
+    <t>0.6831426130539795</t>
+  </si>
+  <si>
+    <t>0.7247321649036378</t>
+  </si>
+  <si>
+    <t>0.71076171788751</t>
   </si>
   <si>
     <t>0.47409961685823754</t>
@@ -1753,6 +1843,36 @@
     <t>0.6230120104035951</t>
   </si>
   <si>
+    <t>0.046660941208647805</t>
+  </si>
+  <si>
+    <t>0.03763167094386289</t>
+  </si>
+  <si>
+    <t>0.03098230664704389</t>
+  </si>
+  <si>
+    <t>0.017168507532233</t>
+  </si>
+  <si>
+    <t>0.03528513346610845</t>
+  </si>
+  <si>
+    <t>0.032923089486773846</t>
+  </si>
+  <si>
+    <t>0.044545384848100215</t>
+  </si>
+  <si>
+    <t>0.027428753139136428</t>
+  </si>
+  <si>
+    <t>0.030591804536601815</t>
+  </si>
+  <si>
+    <t>0.018456662298060908</t>
+  </si>
+  <si>
     <t>0.03351875148794929</t>
   </si>
   <si>
@@ -1813,34 +1933,34 @@
     <t>0.018908752831682644</t>
   </si>
   <si>
-    <t>0.6213553979511426</t>
-  </si>
-  <si>
-    <t>0.4899889630715229</t>
-  </si>
-  <si>
-    <t>0.6463522841632294</t>
-  </si>
-  <si>
-    <t>0.6518604553825549</t>
-  </si>
-  <si>
-    <t>0.6686218770019218</t>
-  </si>
-  <si>
-    <t>0.6685636816792258</t>
-  </si>
-  <si>
-    <t>0.700125392033685</t>
-  </si>
-  <si>
-    <t>0.6892963850746301</t>
-  </si>
-  <si>
-    <t>0.6749205922426329</t>
-  </si>
-  <si>
-    <t>0.6666912809810945</t>
+    <t>0.5743861845378528</t>
+  </si>
+  <si>
+    <t>0.5516285695698526</t>
+  </si>
+  <si>
+    <t>0.6145438222421726</t>
+  </si>
+  <si>
+    <t>0.712280704300357</t>
+  </si>
+  <si>
+    <t>0.6307765869823392</t>
+  </si>
+  <si>
+    <t>0.6522079070068043</t>
+  </si>
+  <si>
+    <t>0.6901693132406026</t>
+  </si>
+  <si>
+    <t>0.7049141137705308</t>
+  </si>
+  <si>
+    <t>0.7429764898850119</t>
+  </si>
+  <si>
+    <t>0.7032998888661122</t>
   </si>
   <si>
     <t>0.38460639569109334</t>
@@ -1903,34 +2023,34 @@
     <t>0.609543300857332</t>
   </si>
   <si>
-    <t>0.5267787767787767</t>
-  </si>
-  <si>
-    <t>0.728511574421279</t>
-  </si>
-  <si>
-    <t>0.6198048600519802</t>
-  </si>
-  <si>
-    <t>0.6302951124200409</t>
-  </si>
-  <si>
-    <t>0.6074555381963567</t>
-  </si>
-  <si>
-    <t>0.6710048934264181</t>
-  </si>
-  <si>
-    <t>0.6568904050648472</t>
-  </si>
-  <si>
-    <t>0.6770426136189549</t>
-  </si>
-  <si>
-    <t>0.706430861923869</t>
-  </si>
-  <si>
-    <t>0.7234194786313549</t>
+    <t>0.5041506439067416</t>
+  </si>
+  <si>
+    <t>0.612261321699524</t>
+  </si>
+  <si>
+    <t>0.6619521535660727</t>
+  </si>
+  <si>
+    <t>0.6427849342840795</t>
+  </si>
+  <si>
+    <t>0.665230760703748</t>
+  </si>
+  <si>
+    <t>0.6795181986506826</t>
+  </si>
+  <si>
+    <t>0.7064589614982231</t>
+  </si>
+  <si>
+    <t>0.6779326824773058</t>
+  </si>
+  <si>
+    <t>0.7186588714094821</t>
+  </si>
+  <si>
+    <t>0.7180953581611836</t>
   </si>
   <si>
     <t>0.37992667992667994</t>
@@ -1993,34 +2113,34 @@
     <t>0.6296620652819319</t>
   </si>
   <si>
-    <t>0.5665527320613112</t>
-  </si>
-  <si>
-    <t>0.5365240877899526</t>
-  </si>
-  <si>
-    <t>0.6170305675975318</t>
-  </si>
-  <si>
-    <t>0.6379221820517836</t>
-  </si>
-  <si>
-    <t>0.6329454371291237</t>
-  </si>
-  <si>
-    <t>0.6642306142008346</t>
-  </si>
-  <si>
-    <t>0.6771424566507931</t>
-  </si>
-  <si>
-    <t>0.6828152715320387</t>
-  </si>
-  <si>
-    <t>0.6880209461297971</t>
-  </si>
-  <si>
-    <t>0.6920292139231075</t>
+    <t>0.5199022877108009</t>
+  </si>
+  <si>
+    <t>0.5767947209570441</t>
+  </si>
+  <si>
+    <t>0.6342529158150425</t>
+  </si>
+  <si>
+    <t>0.6738534938703242</t>
+  </si>
+  <si>
+    <t>0.6463319437388763</t>
+  </si>
+  <si>
+    <t>0.6497061876874903</t>
+  </si>
+  <si>
+    <t>0.6952238235205495</t>
+  </si>
+  <si>
+    <t>0.6883351704365095</t>
+  </si>
+  <si>
+    <t>0.7287176283101944</t>
+  </si>
+  <si>
+    <t>0.7086370849363227</t>
   </si>
   <si>
     <t>0.3718686868686869</t>
@@ -2083,34 +2203,34 @@
     <t>0.6141594253087902</t>
   </si>
   <si>
-    <t>0.5296867990766835</t>
-  </si>
-  <si>
-    <t>0.6242438241471729</t>
-  </si>
-  <si>
-    <t>0.617956392321377</t>
-  </si>
-  <si>
-    <t>0.637498485970854</t>
-  </si>
-  <si>
-    <t>0.6209015717252045</t>
-  </si>
-  <si>
-    <t>0.6683390087045087</t>
-  </si>
-  <si>
-    <t>0.663465401091975</t>
-  </si>
-  <si>
-    <t>0.6805683617382865</t>
-  </si>
-  <si>
-    <t>0.6974661705069423</t>
-  </si>
-  <si>
-    <t>0.7037089088403928</t>
+    <t>0.5153496579254921</t>
+  </si>
+  <si>
+    <t>0.5974586484285151</t>
+  </si>
+  <si>
+    <t>0.6527910148296794</t>
+  </si>
+  <si>
+    <t>0.657680056994102</t>
+  </si>
+  <si>
+    <t>0.6572608916532414</t>
+  </si>
+  <si>
+    <t>0.6626449996837149</t>
+  </si>
+  <si>
+    <t>0.6988983996153927</t>
+  </si>
+  <si>
+    <t>0.6833351303000305</t>
+  </si>
+  <si>
+    <t>0.7246803195414374</t>
+  </si>
+  <si>
+    <t>0.7106964458430317</t>
   </si>
   <si>
     <t>0.4699566475589968</t>
@@ -2631,70 +2751,70 @@
         <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="I2" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>219</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>249</v>
       </c>
       <c r="L2" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="M2" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="N2" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="O2" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="P2" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="Q2" t="s">
-        <v>69</v>
+        <v>429</v>
       </c>
       <c r="R2" t="s">
-        <v>429</v>
+        <v>459</v>
       </c>
       <c r="S2" t="s">
-        <v>459</v>
+        <v>489</v>
       </c>
       <c r="T2" t="s">
-        <v>489</v>
+        <v>519</v>
       </c>
       <c r="U2" t="s">
-        <v>519</v>
+        <v>549</v>
       </c>
       <c r="V2" t="s">
-        <v>549</v>
+        <v>579</v>
       </c>
       <c r="W2" t="s">
-        <v>69</v>
+        <v>609</v>
       </c>
       <c r="X2" t="s">
-        <v>599</v>
+        <v>639</v>
       </c>
       <c r="Y2" t="s">
-        <v>629</v>
+        <v>669</v>
       </c>
       <c r="Z2" t="s">
-        <v>659</v>
+        <v>699</v>
       </c>
       <c r="AA2" t="s">
-        <v>689</v>
+        <v>729</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -2711,73 +2831,73 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="H3" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="I3" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="J3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>250</v>
       </c>
       <c r="L3" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="M3" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="N3" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="O3" t="s">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="P3" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="Q3" t="s">
-        <v>69</v>
+        <v>430</v>
       </c>
       <c r="R3" t="s">
-        <v>430</v>
+        <v>460</v>
       </c>
       <c r="S3" t="s">
-        <v>460</v>
+        <v>490</v>
       </c>
       <c r="T3" t="s">
-        <v>490</v>
+        <v>520</v>
       </c>
       <c r="U3" t="s">
-        <v>520</v>
+        <v>550</v>
       </c>
       <c r="V3" t="s">
-        <v>550</v>
+        <v>580</v>
       </c>
       <c r="W3" t="s">
-        <v>69</v>
+        <v>610</v>
       </c>
       <c r="X3" t="s">
-        <v>600</v>
+        <v>640</v>
       </c>
       <c r="Y3" t="s">
-        <v>630</v>
+        <v>670</v>
       </c>
       <c r="Z3" t="s">
-        <v>660</v>
+        <v>700</v>
       </c>
       <c r="AA3" t="s">
-        <v>690</v>
+        <v>730</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -2794,73 +2914,73 @@
         <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="H4" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="I4" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="J4" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="K4" t="s">
-        <v>69</v>
+        <v>251</v>
       </c>
       <c r="L4" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="M4" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="N4" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="O4" t="s">
-        <v>351</v>
+        <v>371</v>
       </c>
       <c r="P4" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="Q4" t="s">
-        <v>69</v>
+        <v>431</v>
       </c>
       <c r="R4" t="s">
-        <v>431</v>
+        <v>461</v>
       </c>
       <c r="S4" t="s">
-        <v>461</v>
+        <v>491</v>
       </c>
       <c r="T4" t="s">
-        <v>491</v>
+        <v>521</v>
       </c>
       <c r="U4" t="s">
-        <v>521</v>
+        <v>551</v>
       </c>
       <c r="V4" t="s">
-        <v>551</v>
+        <v>581</v>
       </c>
       <c r="W4" t="s">
-        <v>69</v>
+        <v>611</v>
       </c>
       <c r="X4" t="s">
-        <v>601</v>
+        <v>641</v>
       </c>
       <c r="Y4" t="s">
-        <v>631</v>
+        <v>671</v>
       </c>
       <c r="Z4" t="s">
-        <v>661</v>
+        <v>701</v>
       </c>
       <c r="AA4" t="s">
-        <v>691</v>
+        <v>731</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -2877,73 +2997,73 @@
         <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="H5" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="I5" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="J5" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="K5" t="s">
-        <v>69</v>
+        <v>252</v>
       </c>
       <c r="L5" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="M5" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="N5" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="O5" t="s">
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="P5" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="Q5" t="s">
-        <v>69</v>
+        <v>432</v>
       </c>
       <c r="R5" t="s">
-        <v>432</v>
+        <v>462</v>
       </c>
       <c r="S5" t="s">
-        <v>462</v>
+        <v>492</v>
       </c>
       <c r="T5" t="s">
-        <v>492</v>
+        <v>522</v>
       </c>
       <c r="U5" t="s">
-        <v>522</v>
+        <v>552</v>
       </c>
       <c r="V5" t="s">
-        <v>552</v>
+        <v>582</v>
       </c>
       <c r="W5" t="s">
-        <v>69</v>
+        <v>612</v>
       </c>
       <c r="X5" t="s">
-        <v>602</v>
+        <v>642</v>
       </c>
       <c r="Y5" t="s">
-        <v>632</v>
+        <v>672</v>
       </c>
       <c r="Z5" t="s">
-        <v>662</v>
+        <v>702</v>
       </c>
       <c r="AA5" t="s">
-        <v>692</v>
+        <v>732</v>
       </c>
     </row>
     <row r="6" spans="1:27">
@@ -2960,73 +3080,73 @@
         <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="H6" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="I6" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="J6" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="K6" t="s">
-        <v>69</v>
+        <v>253</v>
       </c>
       <c r="L6" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="M6" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="N6" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="O6" t="s">
-        <v>353</v>
+        <v>373</v>
       </c>
       <c r="P6" t="s">
-        <v>383</v>
+        <v>403</v>
       </c>
       <c r="Q6" t="s">
-        <v>69</v>
+        <v>433</v>
       </c>
       <c r="R6" t="s">
-        <v>433</v>
+        <v>463</v>
       </c>
       <c r="S6" t="s">
-        <v>463</v>
+        <v>493</v>
       </c>
       <c r="T6" t="s">
-        <v>493</v>
+        <v>523</v>
       </c>
       <c r="U6" t="s">
-        <v>523</v>
+        <v>553</v>
       </c>
       <c r="V6" t="s">
-        <v>553</v>
+        <v>583</v>
       </c>
       <c r="W6" t="s">
-        <v>69</v>
+        <v>613</v>
       </c>
       <c r="X6" t="s">
-        <v>603</v>
+        <v>643</v>
       </c>
       <c r="Y6" t="s">
-        <v>633</v>
+        <v>673</v>
       </c>
       <c r="Z6" t="s">
-        <v>663</v>
+        <v>703</v>
       </c>
       <c r="AA6" t="s">
-        <v>693</v>
+        <v>733</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -3043,73 +3163,73 @@
         <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="G7" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="H7" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="I7" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="J7" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="K7" t="s">
-        <v>69</v>
+        <v>254</v>
       </c>
       <c r="L7" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="M7" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="N7" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="O7" t="s">
-        <v>354</v>
+        <v>374</v>
       </c>
       <c r="P7" t="s">
-        <v>384</v>
+        <v>404</v>
       </c>
       <c r="Q7" t="s">
-        <v>69</v>
+        <v>434</v>
       </c>
       <c r="R7" t="s">
-        <v>434</v>
+        <v>464</v>
       </c>
       <c r="S7" t="s">
-        <v>464</v>
+        <v>494</v>
       </c>
       <c r="T7" t="s">
-        <v>494</v>
+        <v>524</v>
       </c>
       <c r="U7" t="s">
-        <v>524</v>
+        <v>554</v>
       </c>
       <c r="V7" t="s">
-        <v>554</v>
+        <v>584</v>
       </c>
       <c r="W7" t="s">
-        <v>69</v>
+        <v>614</v>
       </c>
       <c r="X7" t="s">
-        <v>604</v>
+        <v>644</v>
       </c>
       <c r="Y7" t="s">
-        <v>634</v>
+        <v>674</v>
       </c>
       <c r="Z7" t="s">
-        <v>664</v>
+        <v>704</v>
       </c>
       <c r="AA7" t="s">
-        <v>694</v>
+        <v>734</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -3126,73 +3246,73 @@
         <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G8" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="H8" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="I8" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="J8" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="K8" t="s">
-        <v>69</v>
+        <v>255</v>
       </c>
       <c r="L8" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="M8" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="N8" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="O8" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="P8" t="s">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="Q8" t="s">
-        <v>69</v>
+        <v>435</v>
       </c>
       <c r="R8" t="s">
-        <v>435</v>
+        <v>465</v>
       </c>
       <c r="S8" t="s">
-        <v>465</v>
+        <v>495</v>
       </c>
       <c r="T8" t="s">
-        <v>495</v>
+        <v>525</v>
       </c>
       <c r="U8" t="s">
-        <v>525</v>
+        <v>555</v>
       </c>
       <c r="V8" t="s">
-        <v>555</v>
+        <v>585</v>
       </c>
       <c r="W8" t="s">
-        <v>69</v>
+        <v>615</v>
       </c>
       <c r="X8" t="s">
-        <v>605</v>
+        <v>645</v>
       </c>
       <c r="Y8" t="s">
-        <v>635</v>
+        <v>675</v>
       </c>
       <c r="Z8" t="s">
-        <v>665</v>
+        <v>705</v>
       </c>
       <c r="AA8" t="s">
-        <v>695</v>
+        <v>735</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -3209,73 +3329,73 @@
         <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="G9" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="H9" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I9" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="J9" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>256</v>
       </c>
       <c r="L9" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="M9" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="N9" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="O9" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="P9" t="s">
-        <v>386</v>
+        <v>406</v>
       </c>
       <c r="Q9" t="s">
-        <v>69</v>
+        <v>436</v>
       </c>
       <c r="R9" t="s">
-        <v>436</v>
+        <v>466</v>
       </c>
       <c r="S9" t="s">
-        <v>466</v>
+        <v>496</v>
       </c>
       <c r="T9" t="s">
-        <v>496</v>
+        <v>526</v>
       </c>
       <c r="U9" t="s">
-        <v>526</v>
+        <v>556</v>
       </c>
       <c r="V9" t="s">
-        <v>556</v>
+        <v>586</v>
       </c>
       <c r="W9" t="s">
-        <v>69</v>
+        <v>616</v>
       </c>
       <c r="X9" t="s">
-        <v>606</v>
+        <v>646</v>
       </c>
       <c r="Y9" t="s">
-        <v>636</v>
+        <v>676</v>
       </c>
       <c r="Z9" t="s">
-        <v>666</v>
+        <v>706</v>
       </c>
       <c r="AA9" t="s">
-        <v>696</v>
+        <v>736</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -3292,73 +3412,73 @@
         <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="G10" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="H10" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="I10" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="J10" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>257</v>
       </c>
       <c r="L10" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="M10" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="N10" t="s">
-        <v>327</v>
+        <v>347</v>
       </c>
       <c r="O10" t="s">
-        <v>357</v>
+        <v>377</v>
       </c>
       <c r="P10" t="s">
-        <v>387</v>
+        <v>407</v>
       </c>
       <c r="Q10" t="s">
-        <v>69</v>
+        <v>437</v>
       </c>
       <c r="R10" t="s">
-        <v>437</v>
+        <v>467</v>
       </c>
       <c r="S10" t="s">
-        <v>467</v>
+        <v>497</v>
       </c>
       <c r="T10" t="s">
-        <v>497</v>
+        <v>527</v>
       </c>
       <c r="U10" t="s">
-        <v>527</v>
+        <v>557</v>
       </c>
       <c r="V10" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="W10" t="s">
-        <v>69</v>
+        <v>617</v>
       </c>
       <c r="X10" t="s">
-        <v>607</v>
+        <v>647</v>
       </c>
       <c r="Y10" t="s">
-        <v>637</v>
+        <v>677</v>
       </c>
       <c r="Z10" t="s">
-        <v>667</v>
+        <v>707</v>
       </c>
       <c r="AA10" t="s">
-        <v>697</v>
+        <v>737</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -3375,73 +3495,73 @@
         <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="G11" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="H11" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="I11" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="J11" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>258</v>
       </c>
       <c r="L11" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="M11" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="N11" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
       <c r="O11" t="s">
-        <v>358</v>
+        <v>378</v>
       </c>
       <c r="P11" t="s">
-        <v>388</v>
+        <v>408</v>
       </c>
       <c r="Q11" t="s">
-        <v>69</v>
+        <v>438</v>
       </c>
       <c r="R11" t="s">
-        <v>438</v>
+        <v>468</v>
       </c>
       <c r="S11" t="s">
-        <v>468</v>
+        <v>498</v>
       </c>
       <c r="T11" t="s">
-        <v>498</v>
+        <v>528</v>
       </c>
       <c r="U11" t="s">
-        <v>528</v>
+        <v>558</v>
       </c>
       <c r="V11" t="s">
-        <v>558</v>
+        <v>588</v>
       </c>
       <c r="W11" t="s">
-        <v>69</v>
+        <v>618</v>
       </c>
       <c r="X11" t="s">
-        <v>608</v>
+        <v>648</v>
       </c>
       <c r="Y11" t="s">
-        <v>638</v>
+        <v>678</v>
       </c>
       <c r="Z11" t="s">
-        <v>668</v>
+        <v>708</v>
       </c>
       <c r="AA11" t="s">
-        <v>698</v>
+        <v>738</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -3458,73 +3578,73 @@
         <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="G12" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="H12" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="I12" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="J12" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="K12" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="L12" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="M12" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="N12" t="s">
-        <v>329</v>
+        <v>349</v>
       </c>
       <c r="O12" t="s">
-        <v>359</v>
+        <v>379</v>
       </c>
       <c r="P12" t="s">
-        <v>389</v>
+        <v>409</v>
       </c>
       <c r="Q12" t="s">
-        <v>409</v>
+        <v>439</v>
       </c>
       <c r="R12" t="s">
-        <v>439</v>
+        <v>469</v>
       </c>
       <c r="S12" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="T12" t="s">
-        <v>499</v>
+        <v>529</v>
       </c>
       <c r="U12" t="s">
-        <v>529</v>
+        <v>559</v>
       </c>
       <c r="V12" t="s">
-        <v>559</v>
+        <v>589</v>
       </c>
       <c r="W12" t="s">
-        <v>579</v>
+        <v>619</v>
       </c>
       <c r="X12" t="s">
-        <v>609</v>
+        <v>649</v>
       </c>
       <c r="Y12" t="s">
-        <v>639</v>
+        <v>679</v>
       </c>
       <c r="Z12" t="s">
-        <v>669</v>
+        <v>709</v>
       </c>
       <c r="AA12" t="s">
-        <v>699</v>
+        <v>739</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -3541,73 +3661,73 @@
         <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G13" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="H13" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="I13" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="J13" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="K13" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="L13" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="M13" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="N13" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="O13" t="s">
-        <v>360</v>
+        <v>380</v>
       </c>
       <c r="P13" t="s">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="Q13" t="s">
-        <v>410</v>
+        <v>440</v>
       </c>
       <c r="R13" t="s">
-        <v>440</v>
+        <v>470</v>
       </c>
       <c r="S13" t="s">
-        <v>470</v>
+        <v>500</v>
       </c>
       <c r="T13" t="s">
-        <v>500</v>
+        <v>530</v>
       </c>
       <c r="U13" t="s">
-        <v>530</v>
+        <v>560</v>
       </c>
       <c r="V13" t="s">
-        <v>560</v>
+        <v>590</v>
       </c>
       <c r="W13" t="s">
-        <v>580</v>
+        <v>620</v>
       </c>
       <c r="X13" t="s">
-        <v>610</v>
+        <v>650</v>
       </c>
       <c r="Y13" t="s">
-        <v>640</v>
+        <v>680</v>
       </c>
       <c r="Z13" t="s">
-        <v>670</v>
+        <v>710</v>
       </c>
       <c r="AA13" t="s">
-        <v>700</v>
+        <v>740</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -3624,73 +3744,73 @@
         <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="G14" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="H14" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="I14" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="J14" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="K14" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="L14" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="M14" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="N14" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="O14" t="s">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="P14" t="s">
-        <v>391</v>
+        <v>411</v>
       </c>
       <c r="Q14" t="s">
-        <v>411</v>
+        <v>441</v>
       </c>
       <c r="R14" t="s">
-        <v>441</v>
+        <v>471</v>
       </c>
       <c r="S14" t="s">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="T14" t="s">
-        <v>501</v>
+        <v>531</v>
       </c>
       <c r="U14" t="s">
-        <v>531</v>
+        <v>561</v>
       </c>
       <c r="V14" t="s">
-        <v>561</v>
+        <v>591</v>
       </c>
       <c r="W14" t="s">
-        <v>581</v>
+        <v>621</v>
       </c>
       <c r="X14" t="s">
-        <v>611</v>
+        <v>651</v>
       </c>
       <c r="Y14" t="s">
-        <v>641</v>
+        <v>681</v>
       </c>
       <c r="Z14" t="s">
-        <v>671</v>
+        <v>711</v>
       </c>
       <c r="AA14" t="s">
-        <v>701</v>
+        <v>741</v>
       </c>
     </row>
     <row r="15" spans="1:27">
@@ -3707,73 +3827,73 @@
         <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="G15" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="H15" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="I15" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="J15" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="K15" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="L15" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="M15" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="N15" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="O15" t="s">
-        <v>362</v>
+        <v>382</v>
       </c>
       <c r="P15" t="s">
-        <v>392</v>
+        <v>412</v>
       </c>
       <c r="Q15" t="s">
-        <v>412</v>
+        <v>442</v>
       </c>
       <c r="R15" t="s">
-        <v>442</v>
+        <v>472</v>
       </c>
       <c r="S15" t="s">
-        <v>472</v>
+        <v>502</v>
       </c>
       <c r="T15" t="s">
-        <v>502</v>
+        <v>532</v>
       </c>
       <c r="U15" t="s">
-        <v>532</v>
+        <v>562</v>
       </c>
       <c r="V15" t="s">
-        <v>562</v>
+        <v>592</v>
       </c>
       <c r="W15" t="s">
-        <v>582</v>
+        <v>622</v>
       </c>
       <c r="X15" t="s">
-        <v>612</v>
+        <v>652</v>
       </c>
       <c r="Y15" t="s">
-        <v>642</v>
+        <v>682</v>
       </c>
       <c r="Z15" t="s">
-        <v>672</v>
+        <v>712</v>
       </c>
       <c r="AA15" t="s">
-        <v>702</v>
+        <v>742</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -3790,73 +3910,73 @@
         <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="F16" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="G16" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="H16" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="I16" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="J16" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="K16" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="L16" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="M16" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="N16" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="O16" t="s">
-        <v>363</v>
+        <v>383</v>
       </c>
       <c r="P16" t="s">
-        <v>393</v>
+        <v>413</v>
       </c>
       <c r="Q16" t="s">
-        <v>413</v>
+        <v>443</v>
       </c>
       <c r="R16" t="s">
-        <v>443</v>
+        <v>473</v>
       </c>
       <c r="S16" t="s">
-        <v>473</v>
+        <v>503</v>
       </c>
       <c r="T16" t="s">
-        <v>503</v>
+        <v>533</v>
       </c>
       <c r="U16" t="s">
-        <v>533</v>
+        <v>563</v>
       </c>
       <c r="V16" t="s">
-        <v>563</v>
+        <v>593</v>
       </c>
       <c r="W16" t="s">
-        <v>583</v>
+        <v>623</v>
       </c>
       <c r="X16" t="s">
-        <v>613</v>
+        <v>653</v>
       </c>
       <c r="Y16" t="s">
-        <v>643</v>
+        <v>683</v>
       </c>
       <c r="Z16" t="s">
-        <v>673</v>
+        <v>713</v>
       </c>
       <c r="AA16" t="s">
-        <v>703</v>
+        <v>743</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -3873,73 +3993,73 @@
         <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="H17" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="I17" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="J17" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="K17" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="L17" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="M17" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="N17" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="O17" t="s">
-        <v>364</v>
+        <v>384</v>
       </c>
       <c r="P17" t="s">
-        <v>394</v>
+        <v>414</v>
       </c>
       <c r="Q17" t="s">
-        <v>414</v>
+        <v>444</v>
       </c>
       <c r="R17" t="s">
-        <v>444</v>
+        <v>474</v>
       </c>
       <c r="S17" t="s">
-        <v>474</v>
+        <v>504</v>
       </c>
       <c r="T17" t="s">
-        <v>504</v>
+        <v>534</v>
       </c>
       <c r="U17" t="s">
-        <v>534</v>
+        <v>564</v>
       </c>
       <c r="V17" t="s">
-        <v>564</v>
+        <v>594</v>
       </c>
       <c r="W17" t="s">
-        <v>584</v>
+        <v>624</v>
       </c>
       <c r="X17" t="s">
-        <v>614</v>
+        <v>654</v>
       </c>
       <c r="Y17" t="s">
-        <v>644</v>
+        <v>684</v>
       </c>
       <c r="Z17" t="s">
-        <v>674</v>
+        <v>714</v>
       </c>
       <c r="AA17" t="s">
-        <v>704</v>
+        <v>744</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -3956,73 +4076,73 @@
         <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="F18" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="G18" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="H18" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="I18" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="J18" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="K18" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="L18" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="M18" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="N18" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="O18" t="s">
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="P18" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="Q18" t="s">
-        <v>415</v>
+        <v>445</v>
       </c>
       <c r="R18" t="s">
-        <v>445</v>
+        <v>475</v>
       </c>
       <c r="S18" t="s">
-        <v>475</v>
+        <v>505</v>
       </c>
       <c r="T18" t="s">
-        <v>505</v>
+        <v>535</v>
       </c>
       <c r="U18" t="s">
-        <v>535</v>
+        <v>565</v>
       </c>
       <c r="V18" t="s">
-        <v>565</v>
+        <v>595</v>
       </c>
       <c r="W18" t="s">
-        <v>585</v>
+        <v>625</v>
       </c>
       <c r="X18" t="s">
-        <v>615</v>
+        <v>655</v>
       </c>
       <c r="Y18" t="s">
-        <v>645</v>
+        <v>685</v>
       </c>
       <c r="Z18" t="s">
-        <v>675</v>
+        <v>715</v>
       </c>
       <c r="AA18" t="s">
-        <v>705</v>
+        <v>745</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -4039,73 +4159,73 @@
         <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="G19" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="H19" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="I19" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="J19" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="K19" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="L19" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="M19" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="N19" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
       <c r="O19" t="s">
-        <v>366</v>
+        <v>386</v>
       </c>
       <c r="P19" t="s">
-        <v>396</v>
+        <v>416</v>
       </c>
       <c r="Q19" t="s">
-        <v>416</v>
+        <v>446</v>
       </c>
       <c r="R19" t="s">
-        <v>446</v>
+        <v>476</v>
       </c>
       <c r="S19" t="s">
-        <v>476</v>
+        <v>506</v>
       </c>
       <c r="T19" t="s">
-        <v>506</v>
+        <v>536</v>
       </c>
       <c r="U19" t="s">
-        <v>536</v>
+        <v>566</v>
       </c>
       <c r="V19" t="s">
-        <v>566</v>
+        <v>596</v>
       </c>
       <c r="W19" t="s">
-        <v>586</v>
+        <v>626</v>
       </c>
       <c r="X19" t="s">
-        <v>616</v>
+        <v>656</v>
       </c>
       <c r="Y19" t="s">
-        <v>646</v>
+        <v>686</v>
       </c>
       <c r="Z19" t="s">
-        <v>676</v>
+        <v>716</v>
       </c>
       <c r="AA19" t="s">
-        <v>706</v>
+        <v>746</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -4122,73 +4242,73 @@
         <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="F20" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="G20" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="H20" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="I20" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="J20" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="K20" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="L20" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="M20" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="N20" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="O20" t="s">
-        <v>367</v>
+        <v>387</v>
       </c>
       <c r="P20" t="s">
-        <v>397</v>
+        <v>417</v>
       </c>
       <c r="Q20" t="s">
-        <v>417</v>
+        <v>447</v>
       </c>
       <c r="R20" t="s">
-        <v>447</v>
+        <v>477</v>
       </c>
       <c r="S20" t="s">
-        <v>477</v>
+        <v>507</v>
       </c>
       <c r="T20" t="s">
-        <v>507</v>
+        <v>537</v>
       </c>
       <c r="U20" t="s">
-        <v>537</v>
+        <v>567</v>
       </c>
       <c r="V20" t="s">
-        <v>567</v>
+        <v>597</v>
       </c>
       <c r="W20" t="s">
-        <v>587</v>
+        <v>627</v>
       </c>
       <c r="X20" t="s">
-        <v>617</v>
+        <v>657</v>
       </c>
       <c r="Y20" t="s">
-        <v>647</v>
+        <v>687</v>
       </c>
       <c r="Z20" t="s">
-        <v>677</v>
+        <v>717</v>
       </c>
       <c r="AA20" t="s">
-        <v>707</v>
+        <v>747</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -4205,73 +4325,73 @@
         <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="G21" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="H21" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="I21" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="J21" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="K21" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="L21" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="M21" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="N21" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="O21" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="P21" t="s">
-        <v>398</v>
+        <v>418</v>
       </c>
       <c r="Q21" t="s">
-        <v>418</v>
+        <v>448</v>
       </c>
       <c r="R21" t="s">
-        <v>448</v>
+        <v>478</v>
       </c>
       <c r="S21" t="s">
-        <v>478</v>
+        <v>508</v>
       </c>
       <c r="T21" t="s">
-        <v>508</v>
+        <v>538</v>
       </c>
       <c r="U21" t="s">
-        <v>538</v>
+        <v>568</v>
       </c>
       <c r="V21" t="s">
-        <v>568</v>
+        <v>598</v>
       </c>
       <c r="W21" t="s">
-        <v>588</v>
+        <v>628</v>
       </c>
       <c r="X21" t="s">
-        <v>618</v>
+        <v>658</v>
       </c>
       <c r="Y21" t="s">
-        <v>648</v>
+        <v>688</v>
       </c>
       <c r="Z21" t="s">
-        <v>678</v>
+        <v>718</v>
       </c>
       <c r="AA21" t="s">
-        <v>708</v>
+        <v>748</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -4288,73 +4408,73 @@
         <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="F22" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="G22" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="H22" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="I22" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="J22" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="K22" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="L22" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="M22" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="N22" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="O22" t="s">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="P22" t="s">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="Q22" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="R22" t="s">
-        <v>449</v>
+        <v>479</v>
       </c>
       <c r="S22" t="s">
-        <v>479</v>
+        <v>509</v>
       </c>
       <c r="T22" t="s">
-        <v>509</v>
+        <v>539</v>
       </c>
       <c r="U22" t="s">
-        <v>539</v>
+        <v>569</v>
       </c>
       <c r="V22" t="s">
-        <v>569</v>
+        <v>599</v>
       </c>
       <c r="W22" t="s">
-        <v>589</v>
+        <v>629</v>
       </c>
       <c r="X22" t="s">
-        <v>619</v>
+        <v>659</v>
       </c>
       <c r="Y22" t="s">
-        <v>649</v>
+        <v>689</v>
       </c>
       <c r="Z22" t="s">
-        <v>679</v>
+        <v>719</v>
       </c>
       <c r="AA22" t="s">
-        <v>709</v>
+        <v>749</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -4371,73 +4491,73 @@
         <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="G23" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="H23" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="I23" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="J23" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="K23" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="L23" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="M23" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="N23" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="O23" t="s">
-        <v>370</v>
+        <v>390</v>
       </c>
       <c r="P23" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="Q23" t="s">
-        <v>420</v>
+        <v>450</v>
       </c>
       <c r="R23" t="s">
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="S23" t="s">
-        <v>480</v>
+        <v>510</v>
       </c>
       <c r="T23" t="s">
-        <v>510</v>
+        <v>540</v>
       </c>
       <c r="U23" t="s">
-        <v>540</v>
+        <v>570</v>
       </c>
       <c r="V23" t="s">
-        <v>570</v>
+        <v>600</v>
       </c>
       <c r="W23" t="s">
-        <v>590</v>
+        <v>630</v>
       </c>
       <c r="X23" t="s">
-        <v>620</v>
+        <v>660</v>
       </c>
       <c r="Y23" t="s">
-        <v>650</v>
+        <v>690</v>
       </c>
       <c r="Z23" t="s">
-        <v>680</v>
+        <v>720</v>
       </c>
       <c r="AA23" t="s">
-        <v>710</v>
+        <v>750</v>
       </c>
     </row>
     <row r="24" spans="1:27">
@@ -4454,73 +4574,73 @@
         <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="F24" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="G24" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="H24" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="I24" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="J24" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="K24" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="L24" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="M24" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="N24" t="s">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="O24" t="s">
-        <v>371</v>
+        <v>391</v>
       </c>
       <c r="P24" t="s">
-        <v>401</v>
+        <v>421</v>
       </c>
       <c r="Q24" t="s">
-        <v>421</v>
+        <v>451</v>
       </c>
       <c r="R24" t="s">
-        <v>451</v>
+        <v>481</v>
       </c>
       <c r="S24" t="s">
-        <v>481</v>
+        <v>511</v>
       </c>
       <c r="T24" t="s">
-        <v>511</v>
+        <v>541</v>
       </c>
       <c r="U24" t="s">
-        <v>541</v>
+        <v>571</v>
       </c>
       <c r="V24" t="s">
-        <v>571</v>
+        <v>601</v>
       </c>
       <c r="W24" t="s">
-        <v>591</v>
+        <v>631</v>
       </c>
       <c r="X24" t="s">
-        <v>621</v>
+        <v>661</v>
       </c>
       <c r="Y24" t="s">
-        <v>651</v>
+        <v>691</v>
       </c>
       <c r="Z24" t="s">
-        <v>681</v>
+        <v>721</v>
       </c>
       <c r="AA24" t="s">
-        <v>711</v>
+        <v>751</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -4537,73 +4657,73 @@
         <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F25" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="G25" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="H25" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="I25" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="J25" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="K25" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="L25" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="M25" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="N25" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="O25" t="s">
-        <v>372</v>
+        <v>392</v>
       </c>
       <c r="P25" t="s">
-        <v>402</v>
+        <v>422</v>
       </c>
       <c r="Q25" t="s">
-        <v>422</v>
+        <v>452</v>
       </c>
       <c r="R25" t="s">
-        <v>452</v>
+        <v>482</v>
       </c>
       <c r="S25" t="s">
-        <v>482</v>
+        <v>512</v>
       </c>
       <c r="T25" t="s">
-        <v>512</v>
+        <v>542</v>
       </c>
       <c r="U25" t="s">
-        <v>542</v>
+        <v>572</v>
       </c>
       <c r="V25" t="s">
-        <v>572</v>
+        <v>602</v>
       </c>
       <c r="W25" t="s">
-        <v>592</v>
+        <v>632</v>
       </c>
       <c r="X25" t="s">
-        <v>622</v>
+        <v>662</v>
       </c>
       <c r="Y25" t="s">
-        <v>652</v>
+        <v>692</v>
       </c>
       <c r="Z25" t="s">
-        <v>682</v>
+        <v>722</v>
       </c>
       <c r="AA25" t="s">
-        <v>712</v>
+        <v>752</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -4620,73 +4740,73 @@
         <v>63</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F26" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="G26" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="H26" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="I26" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="J26" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="K26" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="L26" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="M26" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="N26" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
       <c r="O26" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="P26" t="s">
-        <v>403</v>
+        <v>423</v>
       </c>
       <c r="Q26" t="s">
-        <v>423</v>
+        <v>453</v>
       </c>
       <c r="R26" t="s">
-        <v>453</v>
+        <v>483</v>
       </c>
       <c r="S26" t="s">
-        <v>483</v>
+        <v>513</v>
       </c>
       <c r="T26" t="s">
-        <v>513</v>
+        <v>543</v>
       </c>
       <c r="U26" t="s">
-        <v>543</v>
+        <v>573</v>
       </c>
       <c r="V26" t="s">
-        <v>573</v>
+        <v>603</v>
       </c>
       <c r="W26" t="s">
-        <v>593</v>
+        <v>633</v>
       </c>
       <c r="X26" t="s">
-        <v>623</v>
+        <v>663</v>
       </c>
       <c r="Y26" t="s">
-        <v>653</v>
+        <v>693</v>
       </c>
       <c r="Z26" t="s">
-        <v>683</v>
+        <v>723</v>
       </c>
       <c r="AA26" t="s">
-        <v>713</v>
+        <v>753</v>
       </c>
     </row>
     <row r="27" spans="1:27">
@@ -4703,73 +4823,73 @@
         <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F27" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="G27" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="H27" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="I27" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="J27" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="K27" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="L27" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="M27" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="N27" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="O27" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="P27" t="s">
-        <v>404</v>
+        <v>424</v>
       </c>
       <c r="Q27" t="s">
-        <v>424</v>
+        <v>454</v>
       </c>
       <c r="R27" t="s">
-        <v>454</v>
+        <v>484</v>
       </c>
       <c r="S27" t="s">
-        <v>484</v>
+        <v>514</v>
       </c>
       <c r="T27" t="s">
-        <v>514</v>
+        <v>544</v>
       </c>
       <c r="U27" t="s">
-        <v>544</v>
+        <v>574</v>
       </c>
       <c r="V27" t="s">
-        <v>574</v>
+        <v>604</v>
       </c>
       <c r="W27" t="s">
-        <v>594</v>
+        <v>634</v>
       </c>
       <c r="X27" t="s">
-        <v>624</v>
+        <v>664</v>
       </c>
       <c r="Y27" t="s">
-        <v>654</v>
+        <v>694</v>
       </c>
       <c r="Z27" t="s">
-        <v>684</v>
+        <v>724</v>
       </c>
       <c r="AA27" t="s">
-        <v>714</v>
+        <v>754</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -4786,73 +4906,73 @@
         <v>65</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F28" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="G28" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="H28" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="I28" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="J28" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="K28" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="L28" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="M28" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="N28" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="O28" t="s">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="P28" t="s">
-        <v>405</v>
+        <v>425</v>
       </c>
       <c r="Q28" t="s">
-        <v>425</v>
+        <v>455</v>
       </c>
       <c r="R28" t="s">
-        <v>455</v>
+        <v>485</v>
       </c>
       <c r="S28" t="s">
-        <v>485</v>
+        <v>515</v>
       </c>
       <c r="T28" t="s">
-        <v>515</v>
+        <v>545</v>
       </c>
       <c r="U28" t="s">
-        <v>545</v>
+        <v>575</v>
       </c>
       <c r="V28" t="s">
-        <v>575</v>
+        <v>605</v>
       </c>
       <c r="W28" t="s">
-        <v>595</v>
+        <v>635</v>
       </c>
       <c r="X28" t="s">
-        <v>625</v>
+        <v>665</v>
       </c>
       <c r="Y28" t="s">
-        <v>655</v>
+        <v>695</v>
       </c>
       <c r="Z28" t="s">
-        <v>685</v>
+        <v>725</v>
       </c>
       <c r="AA28" t="s">
-        <v>715</v>
+        <v>755</v>
       </c>
     </row>
     <row r="29" spans="1:27">
@@ -4869,73 +4989,73 @@
         <v>66</v>
       </c>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F29" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="G29" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="H29" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="I29" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="J29" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="K29" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="L29" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="M29" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
       <c r="N29" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="O29" t="s">
-        <v>376</v>
+        <v>396</v>
       </c>
       <c r="P29" t="s">
-        <v>406</v>
+        <v>426</v>
       </c>
       <c r="Q29" t="s">
-        <v>426</v>
+        <v>456</v>
       </c>
       <c r="R29" t="s">
-        <v>456</v>
+        <v>486</v>
       </c>
       <c r="S29" t="s">
-        <v>486</v>
+        <v>516</v>
       </c>
       <c r="T29" t="s">
-        <v>516</v>
+        <v>546</v>
       </c>
       <c r="U29" t="s">
-        <v>546</v>
+        <v>576</v>
       </c>
       <c r="V29" t="s">
-        <v>576</v>
+        <v>606</v>
       </c>
       <c r="W29" t="s">
-        <v>596</v>
+        <v>636</v>
       </c>
       <c r="X29" t="s">
-        <v>626</v>
+        <v>666</v>
       </c>
       <c r="Y29" t="s">
-        <v>656</v>
+        <v>696</v>
       </c>
       <c r="Z29" t="s">
-        <v>686</v>
+        <v>726</v>
       </c>
       <c r="AA29" t="s">
-        <v>716</v>
+        <v>756</v>
       </c>
     </row>
     <row r="30" spans="1:27">
@@ -4952,73 +5072,73 @@
         <v>67</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="F30" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G30" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="H30" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="I30" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="J30" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="K30" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="L30" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
       <c r="M30" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="N30" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="O30" t="s">
-        <v>377</v>
+        <v>397</v>
       </c>
       <c r="P30" t="s">
-        <v>407</v>
+        <v>427</v>
       </c>
       <c r="Q30" t="s">
-        <v>427</v>
+        <v>457</v>
       </c>
       <c r="R30" t="s">
-        <v>457</v>
+        <v>487</v>
       </c>
       <c r="S30" t="s">
-        <v>487</v>
+        <v>517</v>
       </c>
       <c r="T30" t="s">
-        <v>517</v>
+        <v>547</v>
       </c>
       <c r="U30" t="s">
-        <v>547</v>
+        <v>577</v>
       </c>
       <c r="V30" t="s">
-        <v>577</v>
+        <v>607</v>
       </c>
       <c r="W30" t="s">
-        <v>597</v>
+        <v>637</v>
       </c>
       <c r="X30" t="s">
-        <v>627</v>
+        <v>667</v>
       </c>
       <c r="Y30" t="s">
-        <v>657</v>
+        <v>697</v>
       </c>
       <c r="Z30" t="s">
-        <v>687</v>
+        <v>727</v>
       </c>
       <c r="AA30" t="s">
-        <v>717</v>
+        <v>757</v>
       </c>
     </row>
     <row r="31" spans="1:27">
@@ -5035,73 +5155,73 @@
         <v>68</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="G31" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H31" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="I31" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="J31" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="K31" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="L31" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="M31" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="N31" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="O31" t="s">
-        <v>378</v>
+        <v>398</v>
       </c>
       <c r="P31" t="s">
-        <v>408</v>
+        <v>428</v>
       </c>
       <c r="Q31" t="s">
-        <v>428</v>
+        <v>458</v>
       </c>
       <c r="R31" t="s">
-        <v>458</v>
+        <v>488</v>
       </c>
       <c r="S31" t="s">
-        <v>488</v>
+        <v>518</v>
       </c>
       <c r="T31" t="s">
-        <v>518</v>
+        <v>548</v>
       </c>
       <c r="U31" t="s">
-        <v>548</v>
+        <v>578</v>
       </c>
       <c r="V31" t="s">
-        <v>578</v>
+        <v>608</v>
       </c>
       <c r="W31" t="s">
-        <v>598</v>
+        <v>638</v>
       </c>
       <c r="X31" t="s">
-        <v>628</v>
+        <v>668</v>
       </c>
       <c r="Y31" t="s">
-        <v>658</v>
+        <v>698</v>
       </c>
       <c r="Z31" t="s">
-        <v>688</v>
+        <v>728</v>
       </c>
       <c r="AA31" t="s">
-        <v>718</v>
+        <v>758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>